<commit_message>
Modif mineur au excel
</commit_message>
<xml_diff>
--- a/AnalyseDonnéesTp1.xlsx
+++ b/AnalyseDonnéesTp1.xlsx
@@ -519,7 +519,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -542,6 +542,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,7 +826,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1284,16 +1285,16 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="C15" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="22" t="s">
         <v>60</v>
       </c>
       <c r="H15" t="s">
@@ -1892,16 +1893,16 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B37" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2094,32 +2095,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
-      <c r="U1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="V1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="Z1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
@@ -2132,44 +2133,44 @@
       <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" t="s">
+        <v>54</v>
+      </c>
       <c r="U2" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="V2" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="X2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="Y2" t="s">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="Z2" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="AA2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="AC2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
@@ -2182,44 +2183,44 @@
       <c r="I3" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="R3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" t="s">
+        <v>50</v>
+      </c>
       <c r="U3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="V3" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="W3" t="s">
         <v>50</v>
       </c>
       <c r="X3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y3" t="s">
         <v>57</v>
       </c>
-      <c r="Y3" t="s">
-        <v>1</v>
-      </c>
       <c r="Z3" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="AA3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AB3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AC3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
@@ -2232,44 +2233,44 @@
       <c r="I4" s="6" t="s">
         <v>58</v>
       </c>
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" t="s">
+        <v>50</v>
+      </c>
       <c r="U4" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="V4" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="W4" t="s">
         <v>50</v>
       </c>
       <c r="X4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y4" t="s">
         <v>58</v>
       </c>
-      <c r="Y4" t="s">
-        <v>2</v>
-      </c>
       <c r="Z4" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="AA4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AB4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="AC4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
@@ -2282,44 +2283,44 @@
       <c r="I5" s="6" t="s">
         <v>60</v>
       </c>
+      <c r="R5" t="s">
+        <v>20</v>
+      </c>
+      <c r="S5" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" t="s">
+        <v>50</v>
+      </c>
       <c r="U5" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="V5" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="W5" t="s">
         <v>50</v>
       </c>
       <c r="X5" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="Y5" t="s">
-        <v>3</v>
+        <v>59</v>
       </c>
       <c r="Z5" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="AA5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AB5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="AC5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
@@ -2332,44 +2333,44 @@
       <c r="I6" s="6" t="s">
         <v>57</v>
       </c>
+      <c r="R6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S6" t="s">
+        <v>53</v>
+      </c>
+      <c r="T6" t="s">
+        <v>55</v>
+      </c>
       <c r="U6" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="V6" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="W6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="X6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="Y6" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="Z6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="AA6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AC6" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F7" s="4" t="s">
         <v>36</v>
       </c>
@@ -2382,44 +2383,44 @@
       <c r="I7" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="R7" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" t="s">
+        <v>52</v>
+      </c>
       <c r="U7" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="V7" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="W7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Y7" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="Z7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="AA7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB7" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="AC7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
@@ -2432,44 +2433,44 @@
       <c r="I8" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="R8" t="s">
+        <v>40</v>
+      </c>
+      <c r="S8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T8" t="s">
+        <v>50</v>
+      </c>
       <c r="U8" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="V8" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="W8" t="s">
         <v>50</v>
       </c>
       <c r="X8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="Y8" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="Z8" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="AA8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AB8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="AC8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2482,44 +2483,44 @@
       <c r="I9" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="R9" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" t="s">
+        <v>54</v>
+      </c>
       <c r="U9" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="V9" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="W9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="X9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="Y9" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="Z9" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="AA9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" t="s">
         <v>61</v>
       </c>
-      <c r="AC9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2532,44 +2533,44 @@
       <c r="I10" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="R10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S10" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" t="s">
+        <v>50</v>
+      </c>
       <c r="U10" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="V10" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="W10" t="s">
         <v>50</v>
       </c>
       <c r="X10" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="Y10" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="Z10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="AA10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="AC10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
@@ -2582,32 +2583,32 @@
       <c r="I11" s="6" t="s">
         <v>63</v>
       </c>
+      <c r="R11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S11" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11" t="s">
+        <v>52</v>
+      </c>
       <c r="U11" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="V11" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="W11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="Y11" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="7" t="s">
         <v>31</v>
       </c>
@@ -2620,46 +2621,46 @@
       <c r="I12" s="9" t="s">
         <v>61</v>
       </c>
+      <c r="R12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" t="s">
+        <v>52</v>
+      </c>
       <c r="U12" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="V12" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="W12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="X12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V13" t="s">
+        <v>27</v>
+      </c>
+      <c r="W13" t="s">
+        <v>50</v>
+      </c>
+      <c r="X13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y13" t="s">
         <v>63</v>
       </c>
-      <c r="Y12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Y13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -2684,20 +2685,20 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="3"/>
+      <c r="V14" t="s">
+        <v>33</v>
+      </c>
+      <c r="W14" t="s">
+        <v>50</v>
+      </c>
+      <c r="X14" t="s">
+        <v>55</v>
+      </c>
       <c r="Y14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2746,20 +2747,20 @@
       <c r="P15" s="6" t="s">
         <v>56</v>
       </c>
+      <c r="V15" t="s">
+        <v>37</v>
+      </c>
+      <c r="W15" t="s">
+        <v>50</v>
+      </c>
+      <c r="X15" t="s">
+        <v>54</v>
+      </c>
       <c r="Y15" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -2796,20 +2797,20 @@
       <c r="P16" s="6" t="s">
         <v>63</v>
       </c>
+      <c r="V16" t="s">
+        <v>38</v>
+      </c>
+      <c r="W16" t="s">
+        <v>50</v>
+      </c>
+      <c r="X16" t="s">
+        <v>52</v>
+      </c>
       <c r="Y16" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="4" t="s">
         <v>30</v>
       </c>
@@ -2834,20 +2835,20 @@
       <c r="P17" s="9" t="s">
         <v>61</v>
       </c>
+      <c r="V17" t="s">
+        <v>39</v>
+      </c>
+      <c r="W17" t="s">
+        <v>50</v>
+      </c>
+      <c r="X17" t="s">
+        <v>55</v>
+      </c>
       <c r="Y17" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB17" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E18" s="4" t="s">
         <v>36</v>
       </c>
@@ -2860,20 +2861,20 @@
       <c r="H18" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="V18" t="s">
+        <v>44</v>
+      </c>
+      <c r="W18" t="s">
+        <v>50</v>
+      </c>
+      <c r="X18" t="s">
+        <v>55</v>
+      </c>
       <c r="Y18" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="7" t="s">
         <v>41</v>
       </c>
@@ -2887,8 +2888,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -2914,7 +2915,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
@@ -2992,7 +2993,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
@@ -3018,8 +3019,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
         <v>76</v>
       </c>
@@ -3033,7 +3034,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E29" s="7" t="s">
         <v>30</v>
       </c>
@@ -3059,8 +3060,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
         <v>77</v>
       </c>
@@ -3068,7 +3069,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E32" s="7" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Ajout du tp1 de log2810
</commit_message>
<xml_diff>
--- a/AnalyseDonnéesTp1.xlsx
+++ b/AnalyseDonnéesTp1.xlsx
@@ -1,24 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\LOG2810\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\paulc\github\LOG2810\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5D87A6-7365-418C-9100-83CC25B435F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7455"/>
+    <workbookView xWindow="2805" yWindow="3150" windowWidth="10920" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individus" sheetId="1" r:id="rId1"/>
     <sheet name="Cheveux" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -312,9 +319,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -375,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -515,11 +522,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -530,7 +552,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -543,6 +564,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,16 +845,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -844,14 +867,23 @@
       <c r="D1" t="s">
         <v>56</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="22" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -864,23 +896,29 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="22" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -893,31 +931,36 @@
       <c r="D3" t="s">
         <v>58</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="22">
         <f>SUM(I3:L3)</f>
         <v>50</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="22">
         <f>COUNTIF(B:B,"B")</f>
         <v>11</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="22">
         <f>COUNTIF(B:B,"M")</f>
         <v>13</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="22">
         <f>COUNTIF(B:B,"N")</f>
         <v>17</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="22">
         <f>COUNTIF(B:B,"R")</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -930,31 +973,36 @@
       <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="22">
         <f>SUM(I4:L4)</f>
         <v>100</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="22">
         <f>I3*100/50</f>
         <v>22</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="22">
         <f t="shared" ref="J4:L4" si="0">J3*100/50</f>
         <v>26</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="22">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="22">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -967,26 +1015,31 @@
       <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="22" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -999,35 +1052,39 @@
       <c r="D6" t="s">
         <v>56</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="22">
         <f>SUM(I6:M6)</f>
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="22">
         <f>COUNTIF(C:C,"B")</f>
         <v>17</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="22">
         <f>COUNTIF(C:C,"N")</f>
         <v>12</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="22">
         <f>COUNTIF(C:C,"G")</f>
         <v>13</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="22">
         <f>COUNTIF(C:C,"M")</f>
         <v>1</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="22">
         <f>COUNTIF(C:C,"V")</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1040,35 +1097,39 @@
       <c r="D7" t="s">
         <v>56</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="22">
         <f>SUM(I7:M7)</f>
         <v>100</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="22">
         <f>I6*100/50</f>
         <v>34</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="22">
         <f t="shared" ref="J7:M7" si="1">J6*100/50</f>
         <v>24</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="22">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="22">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="22">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1081,38 +1142,39 @@
       <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="22"/>
+      <c r="H8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="P8" t="s">
+      <c r="P8" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="Q8" s="22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1125,51 +1187,51 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="22">
         <f>SUM(I9:Q9)</f>
         <v>50</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="22">
         <f>COUNTIF(D:D,"GI")</f>
         <v>6</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="22">
         <f>COUNTIF(D:D,"GE")</f>
         <v>8</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="22">
         <f>COUNTIF(D:D,"GP")</f>
         <v>4</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="22">
         <f>COUNTIF(D:D,"GC")</f>
         <v>6</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="22">
         <f>COUNTIF(D:D,"GA")</f>
         <v>6</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="22">
         <f>COUNTIF(D:D,"GM")</f>
         <v>7</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="22">
         <f>COUNTIF(D:D,"GB")</f>
         <v>5</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="22">
         <f>COUNTIF(D:D,"GInd")</f>
         <v>5</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="22">
         <f>COUNTIF(D:D,"ER")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1182,47 +1244,48 @@
       <c r="D10" t="s">
         <v>59</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" s="22"/>
+      <c r="H10" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="22">
         <f>I9*100/50</f>
         <v>12</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="22">
         <f t="shared" ref="J10:Q10" si="2">J9*100/50</f>
         <v>16</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="22">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="22">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="22">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="22">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="22">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="22">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="22">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1236,7 +1299,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1250,7 +1313,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1264,7 +1327,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1280,55 +1343,55 @@
       <c r="H14" t="s">
         <v>83</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+    <row r="15" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>60</v>
       </c>
       <c r="H15" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="15">
         <v>2</v>
       </c>
       <c r="J15" t="s">
         <v>85</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="14">
         <v>3</v>
       </c>
       <c r="L15" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="16">
         <v>5</v>
       </c>
       <c r="N15" t="s">
         <v>84</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="17">
         <v>1</v>
       </c>
       <c r="P15" t="s">
         <v>90</v>
       </c>
-      <c r="Q15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q15" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1344,35 +1407,35 @@
       <c r="H16" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="10">
         <v>0</v>
       </c>
       <c r="L16" t="s">
         <v>60</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="20">
         <v>1</v>
       </c>
       <c r="N16" t="s">
         <v>60</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="10">
         <v>0</v>
       </c>
       <c r="P16" t="s">
         <v>60</v>
       </c>
-      <c r="Q16" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1388,35 +1451,35 @@
       <c r="H17" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="19">
         <v>2</v>
       </c>
       <c r="J17" t="s">
         <v>56</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="19">
         <v>1</v>
       </c>
       <c r="L17" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="11">
         <v>0</v>
       </c>
       <c r="N17" t="s">
         <v>56</v>
       </c>
-      <c r="O17" s="20">
+      <c r="O17" s="19">
         <v>1</v>
       </c>
       <c r="P17" t="s">
         <v>56</v>
       </c>
-      <c r="Q17" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1432,35 +1495,35 @@
       <c r="H18" t="s">
         <v>58</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <v>0</v>
       </c>
       <c r="J18" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="11">
         <v>0</v>
       </c>
       <c r="L18" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="20">
+      <c r="M18" s="19">
         <v>1</v>
       </c>
       <c r="N18" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="11">
         <v>0</v>
       </c>
       <c r="P18" t="s">
         <v>58</v>
       </c>
-      <c r="Q18" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1476,35 +1539,35 @@
       <c r="H19" t="s">
         <v>61</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>61</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="19">
         <v>1</v>
       </c>
       <c r="L19" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="20">
+      <c r="M19" s="19">
         <v>1</v>
       </c>
       <c r="N19" t="s">
         <v>61</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="11">
         <v>0</v>
       </c>
       <c r="P19" t="s">
         <v>61</v>
       </c>
-      <c r="Q19" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -1520,35 +1583,35 @@
       <c r="H20" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="11">
         <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>59</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="11">
         <v>0</v>
       </c>
       <c r="L20" t="s">
         <v>59</v>
       </c>
-      <c r="M20" s="20">
+      <c r="M20" s="19">
         <v>1</v>
       </c>
       <c r="N20" t="s">
         <v>59</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="11">
         <v>0</v>
       </c>
       <c r="P20" t="s">
         <v>59</v>
       </c>
-      <c r="Q20" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1564,35 +1627,35 @@
       <c r="H21" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="11">
         <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="11">
         <v>0</v>
       </c>
       <c r="L21" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="20">
+      <c r="M21" s="19">
         <v>1</v>
       </c>
       <c r="N21" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="11">
         <v>0</v>
       </c>
       <c r="P21" t="s">
         <v>57</v>
       </c>
-      <c r="Q21" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1608,35 +1671,35 @@
       <c r="H22" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="19">
         <v>1</v>
       </c>
       <c r="L22" t="s">
         <v>63</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="11">
         <v>0</v>
       </c>
       <c r="N22" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="11">
         <v>0</v>
       </c>
       <c r="P22" t="s">
         <v>63</v>
       </c>
-      <c r="Q22" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1652,35 +1715,35 @@
       <c r="H23" t="s">
         <v>62</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="11">
         <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="11">
         <v>0</v>
       </c>
       <c r="L23" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="11">
         <v>0</v>
       </c>
       <c r="N23" t="s">
         <v>62</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="11">
         <v>0</v>
       </c>
       <c r="P23" t="s">
         <v>62</v>
       </c>
-      <c r="Q23" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1696,35 +1759,35 @@
       <c r="H24" t="s">
         <v>64</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="12">
         <v>0</v>
       </c>
       <c r="J24" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="12">
         <v>0</v>
       </c>
       <c r="L24" t="s">
         <v>64</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M24" s="12">
         <v>0</v>
       </c>
       <c r="N24" t="s">
         <v>64</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="12">
         <v>0</v>
       </c>
       <c r="P24" t="s">
         <v>64</v>
       </c>
-      <c r="Q24" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +1801,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1752,7 +1815,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1766,7 +1829,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1780,7 +1843,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1794,7 +1857,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -1808,7 +1871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -1822,7 +1885,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1899,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1850,7 +1913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1864,7 +1927,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -1878,7 +1941,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -1892,21 +1955,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="22" t="s">
+      <c r="B37" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="21" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1920,7 +1983,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1934,7 +1997,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1948,7 +2011,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1962,7 +2025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1976,7 +2039,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -1990,7 +2053,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -2004,7 +2067,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>21</v>
       </c>
@@ -2018,7 +2081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2032,7 +2095,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -2046,7 +2109,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -2060,7 +2123,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>35</v>
       </c>
@@ -2074,7 +2137,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2090,20 +2153,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC35"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="W25" sqref="W25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F1" s="1" t="s">
         <v>67</v>
       </c>
@@ -2120,7 +2184,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
@@ -2170,7 +2234,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
@@ -2220,7 +2284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
@@ -2270,7 +2334,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
@@ -2320,7 +2384,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F6" s="4" t="s">
         <v>30</v>
       </c>
@@ -2370,7 +2434,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F7" s="4" t="s">
         <v>36</v>
       </c>
@@ -2420,7 +2484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F8" s="4" t="s">
         <v>41</v>
       </c>
@@ -2470,7 +2534,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2520,7 +2584,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2570,7 +2634,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="F11" s="4" t="s">
         <v>18</v>
       </c>
@@ -2608,7 +2672,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="F12" s="7" t="s">
         <v>31</v>
       </c>
@@ -2646,7 +2710,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="V13" t="s">
         <v>27</v>
       </c>
@@ -2660,7 +2724,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>69</v>
       </c>
@@ -2698,7 +2762,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -2760,7 +2824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -2810,7 +2874,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E17" s="4" t="s">
         <v>30</v>
       </c>
@@ -2848,7 +2912,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="E18" s="4" t="s">
         <v>36</v>
       </c>
@@ -2874,7 +2938,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E19" s="7" t="s">
         <v>41</v>
       </c>
@@ -2888,8 +2952,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -2915,7 +2979,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -2965,7 +3029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="7" t="s">
         <v>29</v>
       </c>
@@ -2979,7 +3043,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
@@ -2993,7 +3057,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E26" s="7" t="s">
         <v>24</v>
       </c>
@@ -3019,8 +3083,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="E28" s="1" t="s">
         <v>76</v>
       </c>
@@ -3034,7 +3098,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E29" s="7" t="s">
         <v>30</v>
       </c>
@@ -3060,8 +3124,8 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="E31" s="1" t="s">
         <v>77</v>
       </c>
@@ -3069,7 +3133,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E32" s="7" t="s">
         <v>36</v>
       </c>
@@ -3083,8 +3147,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="34" spans="5:8" x14ac:dyDescent="0.45">
       <c r="E34" s="1" t="s">
         <v>78</v>
       </c>
@@ -3092,7 +3156,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E35" s="7" t="s">
         <v>41</v>
       </c>
@@ -3107,7 +3171,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="F2:I12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:I12">
     <sortCondition ref="H2:H12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>